<commit_message>
add 1 more test cases for CBSSprots SoccerPage
</commit_message>
<xml_diff>
--- a/com.cbssports/src/test/resources/CBSSportsTestData.xlsx
+++ b/com.cbssports/src/test/resources/CBSSportsTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdaziz/IdeaProjects/Team1BootCamp/com.cbssports/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D874D1-4EC8-824F-844D-0459DFA28D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4B1021-C903-B347-BAD9-7768628E9DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" activeTab="2" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>A</t>
   </si>
@@ -92,6 +92,36 @@
   </si>
   <si>
     <t>https://www.viacomcbsprivacy.com/en/donotsell?r=www.cbssports.com#top</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Português (Brasil)</t>
+  </si>
+  <si>
+    <t>Français</t>
+  </si>
+  <si>
+    <t>Español</t>
+  </si>
+  <si>
+    <t>日本</t>
+  </si>
+  <si>
+    <t>©2021 ViacomCBS - Todos los derechos reservados</t>
+  </si>
+  <si>
+    <t>©2021 ViacomCBS - Tous droits réservés</t>
+  </si>
+  <si>
+    <t>Footer</t>
+  </si>
+  <si>
+    <t>©2021 ViacomCBS - Todos os direitos reservados</t>
+  </si>
+  <si>
+    <t>©2021 ViacomCBS - All rights reserved</t>
   </si>
 </sst>
 </file>
@@ -607,40 +637,72 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57A517B4-AB0A-4E50-8324-F3955FA294DA}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="62" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" customWidth="1"/>
+    <col min="3" max="3" width="39.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>